<commit_message>
Modificación de shell, casi completo
</commit_message>
<xml_diff>
--- a/Array con datos.xlsx
+++ b/Array con datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\solid\Desktop\ITC\Semestre3\Estructura Datos\Parcial4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A38F8C0-AAC8-453A-A958-082B5DD25D01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7998F4-1799-4E99-84EB-7C4D3321DFEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CC73EF2D-E2D0-4FCE-A602-9D3F647567A8}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>ORIGINAL</t>
+    <t>j</t>
   </si>
 </sst>
 </file>
@@ -54,7 +54,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -67,8 +67,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9999"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66FF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -106,28 +136,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -136,6 +158,11 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF9999"/>
+      <color rgb="FF66FF99"/>
+      <color rgb="FFCCFFFF"/>
+      <color rgb="FFFFFFCC"/>
+      <color rgb="FFFFCC99"/>
       <color rgb="FFCC99FF"/>
     </mruColors>
   </colors>
@@ -450,139 +477,190 @@
   <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="18" width="7.1796875" customWidth="1"/>
+    <col min="1" max="18" width="5.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="H1" s="2" t="s">
+      <c r="A1">
         <v>0</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+      <c r="N1">
+        <v>13</v>
+      </c>
+      <c r="O1">
+        <v>14</v>
+      </c>
+      <c r="P1">
+        <v>15</v>
+      </c>
+      <c r="Q1">
+        <v>16</v>
+      </c>
+      <c r="R1">
+        <v>17</v>
+      </c>
     </row>
     <row r="2" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="3">
+      <c r="A2" s="1">
+        <v>24</v>
+      </c>
+      <c r="B2" s="4">
+        <v>54</v>
+      </c>
+      <c r="C2" s="5">
+        <v>2</v>
+      </c>
+      <c r="D2" s="6">
+        <v>89</v>
+      </c>
+      <c r="E2" s="7">
+        <v>80</v>
+      </c>
+      <c r="F2" s="8">
+        <v>11</v>
+      </c>
+      <c r="G2" s="2">
         <v>10</v>
       </c>
-      <c r="B2" s="1">
-        <v>54</v>
-      </c>
-      <c r="C2" s="1">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1">
-        <v>89</v>
-      </c>
-      <c r="E2" s="1">
-        <v>80</v>
-      </c>
-      <c r="F2" s="1">
-        <v>89</v>
-      </c>
-      <c r="G2" s="4">
-        <v>24</v>
-      </c>
-      <c r="H2" s="1">
-        <v>2</v>
-      </c>
-      <c r="I2" s="1">
+      <c r="H2" s="4">
+        <v>3</v>
+      </c>
+      <c r="I2" s="5">
         <v>55</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="6">
         <v>65</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K2" s="7">
         <v>5</v>
       </c>
-      <c r="L2" s="1">
+      <c r="L2" s="8">
         <v>70</v>
       </c>
-      <c r="M2" s="4">
+      <c r="M2" s="2">
         <v>45</v>
       </c>
-      <c r="N2" s="1">
+      <c r="N2" s="4">
         <v>88</v>
       </c>
-      <c r="O2" s="1">
-        <v>54</v>
-      </c>
-      <c r="P2" s="1">
-        <v>45</v>
-      </c>
-      <c r="Q2" s="1">
+      <c r="O2" s="5">
+        <v>114</v>
+      </c>
+      <c r="P2" s="6">
+        <v>46</v>
+      </c>
+      <c r="Q2" s="7">
         <v>77</v>
       </c>
-      <c r="R2" s="1">
+      <c r="R2" s="8">
         <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="5" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="3">
+      <c r="A5" s="1">
         <v>10</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="3">
         <v>54</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="3">
         <v>2</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="2">
         <v>89</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="3">
         <v>80</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="3">
         <v>89</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="2">
         <v>24</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="3">
         <v>2</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="3">
         <v>55</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="2">
         <v>65</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="3">
         <v>5</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="3">
         <v>70</v>
       </c>
-      <c r="M5" s="4">
+      <c r="M5" s="2">
         <v>45</v>
       </c>
-      <c r="N5" s="5">
+      <c r="N5" s="3">
         <v>88</v>
       </c>
-      <c r="O5" s="5">
+      <c r="O5" s="3">
         <v>54</v>
       </c>
-      <c r="P5" s="4">
+      <c r="P5" s="2">
         <v>45</v>
       </c>
-      <c r="Q5" s="5">
+      <c r="Q5" s="3">
         <v>77</v>
       </c>
-      <c r="R5" s="5">
+      <c r="R5" s="3">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="H1:K1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>